<commit_message>
Reduced cost and mass FELA
</commit_message>
<xml_diff>
--- a/GameData/WarpPlugin/Parts/Microwave/BeamedPower.xlsx
+++ b/GameData/WarpPlugin/Parts/Microwave/BeamedPower.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\WarpPlugin\Parts\Microwave\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18615" windowHeight="11370"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Transmit</t>
   </si>
@@ -32,9 +27,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Phased Array (Deploable)</t>
-  </si>
-  <si>
     <t>Receive</t>
   </si>
   <si>
@@ -72,12 +64,24 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Phased Array (Deployable)</t>
+  </si>
+  <si>
+    <t>Multi Bandwidth Dish Transceiver (large)</t>
+  </si>
+  <si>
+    <t>Multi Bandwidth Dish Transceiver (medium)</t>
+  </si>
+  <si>
+    <t>Multi Bandwidth Dish Transceiver (shielded)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,7 +419,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -423,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,35 +440,35 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -476,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -487,10 +491,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -513,10 +517,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4.5</v>
@@ -539,10 +543,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>4.5</v>
@@ -565,10 +569,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -580,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>0.5</v>
@@ -591,10 +595,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -606,13 +610,64 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <v>0.15</v>
       </c>
       <c r="H8">
         <v>380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>3500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>